<commit_message>
progress for 1-15 problems updated
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dsa-basics-70\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED98972E-E057-493F-B310-832AA1085982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A604120E-93E3-46A3-B82A-258D3F680652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="107">
   <si>
     <t>No</t>
   </si>
@@ -326,6 +326,21 @@
   </si>
   <si>
     <t>(C*9/5)+32</t>
+  </si>
+  <si>
+    <t>Used πr², float input, exponent operator</t>
+  </si>
+  <si>
+    <t>Used lower(), isalpha(), membership operator(in)</t>
+  </si>
+  <si>
+    <t>Used ord() to convert a character to an ASCII value; validated single-character input</t>
+  </si>
+  <si>
+    <t>Used modulo operator; used logical AND; both conditions must be true</t>
+  </si>
+  <si>
+    <t>Implemented flat slab calculation; used range comparisons; handled negative input; structured increasing conditions</t>
   </si>
 </sst>
 </file>
@@ -669,7 +684,7 @@
   <dimension ref="A1:I71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1007,7 +1022,22 @@
         <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E12" s="1">
+        <v>46079</v>
+      </c>
+      <c r="F12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1021,7 +1051,22 @@
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E13" s="1">
+        <v>46079</v>
+      </c>
+      <c r="F13" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" t="s">
+        <v>88</v>
+      </c>
+      <c r="I13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1035,7 +1080,22 @@
         <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E14" s="1">
+        <v>46079</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H14" t="s">
+        <v>88</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1049,7 +1109,22 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E15" s="1">
+        <v>46079</v>
+      </c>
+      <c r="F15" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" t="s">
+        <v>91</v>
+      </c>
+      <c r="H15" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1063,7 +1138,22 @@
         <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>89</v>
+      </c>
+      <c r="E16" s="1">
+        <v>46079</v>
+      </c>
+      <c r="F16" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" t="s">
+        <v>96</v>
+      </c>
+      <c r="H16" t="s">
+        <v>88</v>
+      </c>
+      <c r="I16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>